<commit_message>
Simulation and Pickup Changes
</commit_message>
<xml_diff>
--- a/samples/rider_details.xlsx
+++ b/samples/rider_details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prash\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prash\Documents\ps_3\backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{870D2666-C879-4791-95AF-3CF71E676388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24DFC4B-0BEF-48CB-AD0C-EF213F33FCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5F42965-60D4-47E8-8E98-BAC9F1DD8F7B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -48,29 +48,71 @@
     <t>currentAvailableBagVolume</t>
   </si>
   <si>
-    <t>Nishant Devan</t>
-  </si>
-  <si>
-    <t>Pratik Gokhale</t>
-  </si>
-  <si>
-    <t>Devansh Agate</t>
-  </si>
-  <si>
-    <t>Aarav Ravel</t>
-  </si>
-  <si>
-    <t>Jagan Sahni</t>
+    <t>Shree</t>
+  </si>
+  <si>
+    <t>Sarthak</t>
+  </si>
+  <si>
+    <t>Sarthak2</t>
+  </si>
+  <si>
+    <t>Arpit</t>
+  </si>
+  <si>
+    <t>Harsh</t>
+  </si>
+  <si>
+    <t>Jagdish</t>
+  </si>
+  <si>
+    <t>Sushant</t>
+  </si>
+  <si>
+    <t>Pranay</t>
+  </si>
+  <si>
+    <t>rider1</t>
+  </si>
+  <si>
+    <t>rider2</t>
+  </si>
+  <si>
+    <t>rider3</t>
+  </si>
+  <si>
+    <t>rider4</t>
+  </si>
+  <si>
+    <t>rider5</t>
+  </si>
+  <si>
+    <t>rider6</t>
+  </si>
+  <si>
+    <t>rider7</t>
+  </si>
+  <si>
+    <t>rider8</t>
+  </si>
+  <si>
+    <t>riderID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -412,105 +454,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154E9F5F-9AF6-4F54-A8F0-74D13D55B269}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="1" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>6127979336</v>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>67.400000000000006</v>
+        <v>9511725963</v>
       </c>
       <c r="D2">
-        <v>67.400000000000006</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <f>80*80*100</f>
+        <v>640000</v>
+      </c>
+      <c r="E2">
+        <f>D2</f>
+        <v>640000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>8917042871</v>
+      <c r="B3" t="s">
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>56.87</v>
+        <v>6239803560</v>
       </c>
       <c r="D3">
-        <v>56.87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" ref="D3:D5" si="0">80*80*100</f>
+        <v>640000</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="1">D3</f>
+        <v>640000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>6801285752</v>
+      <c r="B4" t="s">
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>72.680000000000007</v>
+        <v>1234567890</v>
       </c>
       <c r="D4">
-        <v>72.680000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>640000</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>640000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>6127950667</v>
+      <c r="B5" t="s">
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>47.12</v>
+        <v>3456789123</v>
       </c>
       <c r="D5">
-        <v>47.12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>640000</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>640000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>3457899322</v>
+      </c>
+      <c r="D6">
+        <f>60*60*100</f>
+        <v>360000</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>6127963952</v>
-      </c>
-      <c r="C6">
-        <v>67.22</v>
-      </c>
-      <c r="D6">
-        <v>67.22</v>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>9680518959</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D9" si="2">60*60*100</f>
+        <v>360000</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>6804188859</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>360000</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>9680518923</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>360000</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>360000</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>